<commit_message>
Allow re-runs to update existing records in ES
</commit_message>
<xml_diff>
--- a/CSV2Report/server/ReportData.xlsx
+++ b/CSV2Report/server/ReportData.xlsx
@@ -14,8 +14,42 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Electric Cloud</author>
+  </authors>
+  <commentList>
+    <comment ref="B1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Urvashi S:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+'documentId' is a special  system-recognized column that can be used to uniquely identify a record in ElasticSearch. If a record already exists in ES for the specified documentId for the report object, it will be updated with the data in the row.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="34">
   <si>
     <t>Command to perform an ECHO</t>
   </si>
@@ -32,9 +66,6 @@
     <t>Command to change to a specific directory</t>
   </si>
   <si>
-    <t>Command to grab MS Windows version</t>
-  </si>
-  <si>
     <t>Report Object</t>
   </si>
   <si>
@@ -114,13 +145,19 @@
   </si>
   <si>
     <t>2018-01-14'T'08:45:30.000</t>
+  </si>
+  <si>
+    <t>documentId</t>
+  </si>
+  <si>
+    <t>Updating desc for EC-5 again</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -134,6 +171,25 @@
       <color rgb="FF0000FF"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF2F2F2F"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -162,16 +218,59 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF2F2F2F"/>
+        <name val="Segoe UI"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF0000FF"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
@@ -184,6 +283,23 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:F8" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:F8"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Report Object"/>
+    <tableColumn id="2" name="documentId" dataDxfId="0">
+      <calculatedColumnFormula>ROW(A1)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" name="Commit ID"/>
+    <tableColumn id="4" name="Associated Defect"/>
+    <tableColumn id="5" name="Commit Description"/>
+    <tableColumn id="6" name="Commit Date"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -471,31 +587,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A8"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="16.33203125" customWidth="1"/>
-    <col min="2" max="3" width="26.77734375" customWidth="1"/>
-    <col min="4" max="4" width="36.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="32.44140625" customWidth="1"/>
-    <col min="6" max="6" width="28.6640625" customWidth="1"/>
-    <col min="7" max="7" width="30.109375" customWidth="1"/>
+    <col min="1" max="1" width="19.77734375" customWidth="1"/>
+    <col min="2" max="2" width="13.77734375" customWidth="1"/>
+    <col min="3" max="4" width="26.77734375" customWidth="1"/>
+    <col min="5" max="5" width="36.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="32.44140625" customWidth="1"/>
+    <col min="7" max="7" width="28.6640625" customWidth="1"/>
+    <col min="8" max="8" width="30.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.6">
+    <row r="1" spans="1:6" ht="15.6">
       <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>10</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>9</v>
@@ -503,129 +620,164 @@
       <c r="E1" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:6" ht="15">
       <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="2">
+        <f>ROW(A1)</f>
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
         <v>18</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="2">
+        <f t="shared" ref="B3:B7" si="0">ROW(A2)</f>
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
         <v>19</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D3" t="s">
         <v>11</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="2">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="2">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="2">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="2">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="2">
+        <f>ROW(A7)</f>
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" t="s">
         <v>0</v>
       </c>
-      <c r="E2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" t="s">
-        <v>2</v>
-      </c>
-      <c r="E5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" t="s">
-        <v>3</v>
-      </c>
-      <c r="E6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" t="s">
-        <v>4</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="F8" t="s">
         <v>31</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" t="s">
-        <v>0</v>
-      </c>
-      <c r="E8" t="s">
-        <v>32</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
 </worksheet>
 </file>
 

</xml_diff>